<commit_message>
Upload data for 29 Palms from spring 2022
</commit_message>
<xml_diff>
--- a/data/raw/29Palms_Spr22.xlsx
+++ b/data/raw/29Palms_Spr22.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{EA4BDCC8-E435-4226-ACB8-1ED76C3B0A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53CD79E2-A235-4897-8733-D54F28DBED85}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{EA4BDCC8-E435-4226-ACB8-1ED76C3B0A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A8B4B40-5977-43BB-924E-54FB002B242A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3360" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{349B4CE0-1FB1-4870-898B-07A5C0E5E3C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{349B4CE0-1FB1-4870-898B-07A5C0E5E3C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="to merge with raw_LO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="68">
   <si>
     <t>29_Palms</t>
   </si>
@@ -183,13 +184,70 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Date_Seeded</t>
+  </si>
+  <si>
+    <t>Date_Monitored</t>
+  </si>
+  <si>
+    <t>Recorder_Initials</t>
+  </si>
+  <si>
+    <t>Seed_Mix</t>
+  </si>
+  <si>
+    <t>Species_Code</t>
+  </si>
+  <si>
+    <t>Seedling_Count</t>
+  </si>
+  <si>
+    <t>Average_Height_mm</t>
+  </si>
+  <si>
+    <t>Functional_Group</t>
+  </si>
+  <si>
+    <t>Seeded(Yes/No)</t>
+  </si>
+  <si>
+    <t>Certainty_of_ID(1-3)</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Mulch</t>
+  </si>
+  <si>
+    <t>Pits</t>
+  </si>
+  <si>
+    <t>ConMod</t>
+  </si>
+  <si>
+    <t>Pellets</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +256,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -225,10 +291,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,6 +313,86 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B50D05A7-BF78-3B66-D208-F5B2EB23D7D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9448800" y="419100"/>
+          <a:ext cx="3177540" cy="830580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Sheet1 is the original file I was sent. This tab is to format the columns in a way that they will</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> merge with the rest of the raw master subplot data.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FD93AB-ADDD-4B9D-9B03-DD7C4AE1AE61}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2945,16 +3094,2007 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37386FC8-E60D-4BD1-ABCE-B1EE95A99354}">
+  <dimension ref="A1:N45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M10" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" t="s">
+        <v>4</v>
+      </c>
+      <c r="M14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>4</v>
+      </c>
+      <c r="M20" t="s">
+        <v>4</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>20</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>4</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" t="s">
+        <v>4</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" t="s">
+        <v>4</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
+        <v>27</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" t="s">
+        <v>4</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>29</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>4</v>
+      </c>
+      <c r="M31" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>31</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>4</v>
+      </c>
+      <c r="L32" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>32</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>4</v>
+      </c>
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" t="s">
+        <v>4</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>33</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>4</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>34</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>4</v>
+      </c>
+      <c r="L35" t="s">
+        <v>4</v>
+      </c>
+      <c r="M35" t="s">
+        <v>4</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>35</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>4</v>
+      </c>
+      <c r="L36" t="s">
+        <v>4</v>
+      </c>
+      <c r="M36" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>36</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>4</v>
+      </c>
+      <c r="L37" t="s">
+        <v>4</v>
+      </c>
+      <c r="M37" t="s">
+        <v>4</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1">
+        <v>37</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" t="s">
+        <v>4</v>
+      </c>
+      <c r="M38" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C39" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>38</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" t="s">
+        <v>4</v>
+      </c>
+      <c r="M39" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C40" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>39</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>4</v>
+      </c>
+      <c r="L40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M40" t="s">
+        <v>4</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C41" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>40</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>4</v>
+      </c>
+      <c r="L41" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" t="s">
+        <v>4</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C42" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <v>41</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
+        <v>4</v>
+      </c>
+      <c r="L42" t="s">
+        <v>4</v>
+      </c>
+      <c r="M42" t="s">
+        <v>4</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C43" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>42</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" t="s">
+        <v>4</v>
+      </c>
+      <c r="M43" t="s">
+        <v>4</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <v>43</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>4</v>
+      </c>
+      <c r="L44" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" t="s">
+        <v>4</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="2">
+        <v>44549</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44666</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1">
+        <v>44</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
+        <v>4</v>
+      </c>
+      <c r="L45" t="s">
+        <v>4</v>
+      </c>
+      <c r="M45" t="s">
+        <v>4</v>
+      </c>
+      <c r="N45" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="81398b91-6abb-4fb5-accf-e2304daf6eba">
@@ -2963,6 +5103,15 @@
     <TaxCatchAll xmlns="31062a0d-ede8-4112-b4bb-00a9c1bc8e16"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3206,14 +5355,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D1B0AA3-0B55-4F10-8725-5C78891C5480}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6666D5DF-E7EC-4E86-9632-AF370EF5FEDB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3227,6 +5368,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D1B0AA3-0B55-4F10-8725-5C78891C5480}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>